<commit_message>
Updates to make the USAID data work.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/USDA GFS IMPACT V23.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/USDA GFS IMPACT V23.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="372">
   <si>
     <t>Bananas</t>
   </si>
@@ -1140,6 +1140,57 @@
   </si>
   <si>
     <t>vit_d_µg</t>
+  </si>
+  <si>
+    <t>Australian retention code</t>
+  </si>
+  <si>
+    <t>Retention Description</t>
+  </si>
+  <si>
+    <t>thiamin cooking retention</t>
+  </si>
+  <si>
+    <t>vit b12  cooking retention</t>
+  </si>
+  <si>
+    <t>riboflavin cooking retention</t>
+  </si>
+  <si>
+    <t>niacin cooking retention</t>
+  </si>
+  <si>
+    <t>calcium cooking retention</t>
+  </si>
+  <si>
+    <t>iron cooking retention</t>
+  </si>
+  <si>
+    <t>folate  cooking retention</t>
+  </si>
+  <si>
+    <t>potassium cooking retention</t>
+  </si>
+  <si>
+    <t>magnesium cooking retention</t>
+  </si>
+  <si>
+    <t>phosphorus  cooking retention</t>
+  </si>
+  <si>
+    <t>vitamin c  cooking retention</t>
+  </si>
+  <si>
+    <t>vitamin e  cooking retention</t>
+  </si>
+  <si>
+    <t>zinc  cooking retention</t>
+  </si>
+  <si>
+    <t>vitamin b6 cooking retention</t>
+  </si>
+  <si>
+    <t>vitamin a rae cooking retention</t>
   </si>
 </sst>
 </file>
@@ -2740,10 +2791,10 @@
   <dimension ref="A1:BJ66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AN5" sqref="AN5"/>
+      <selection pane="bottomRight" activeCell="AY6" sqref="AY6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2916,7 +2967,57 @@
       <c r="AS1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AT1" s="39"/>
+      <c r="AT1" s="39" t="s">
+        <v>355</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="AW1" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="AX1" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="AY1" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="AZ1" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="BA1" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="BB1" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="BC1" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="BF1" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="BH1" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="BI1" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="2" spans="1:62" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="125"/>

</xml_diff>